<commit_message>
Add readingExcel.py for Reading Excel files
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -357,13 +357,16 @@
       <c r="A1" t="n">
         <v>56</v>
       </c>
+      <c r="B1" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>43</v>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3">
@@ -372,6 +375,9 @@
           <t>07/31/19</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">

</xml_diff>